<commit_message>
up date code seating  cruise
</commit_message>
<xml_diff>
--- a/CMS.Web/Modules/Sails/Admin/ExportTemplates/TourCommandAndWelcomeBoard.xlsx
+++ b/CMS.Web/Modules/Sails/Admin/ExportTemplates/TourCommandAndWelcomeBoard.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Project\orientalsails\CMS.Web\Modules\Sails\Admin\ExportTemplates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D5A9392D-165A-4AC6-94C1-8C5B20CDB072}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2EA35152-B7DF-4EAC-B0B7-B90E969FC5A9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="679" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="6735" yWindow="1950" windowWidth="17280" windowHeight="8970" tabRatio="679" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tour Command" sheetId="10" r:id="rId1"/>
@@ -20,12 +20,22 @@
     <definedName name="_xlnm.Print_Area" localSheetId="0">'Tour Command'!$A:$K</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="1">'welcome board'!$A$1:$K$6</definedName>
   </definedNames>
-  <calcPr calcId="125725"/>
+  <calcPr calcId="181029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="27">
   <si>
     <t>Driver:</t>
   </si>
@@ -42,15 +52,6 @@
     <t xml:space="preserve">Note: </t>
   </si>
   <si>
-    <t>Day 1</t>
-  </si>
-  <si>
-    <t>Day 2</t>
-  </si>
-  <si>
-    <t>Day 3</t>
-  </si>
-  <si>
     <t>Total:</t>
   </si>
   <si>
@@ -102,9 +103,6 @@
     <t>WELCOME</t>
   </si>
   <si>
-    <t>Guide's Salary                                          Điều hành ký</t>
-  </si>
-  <si>
     <t>HDV hỏi khách có yêu cầu, ăn kiêng chay gì không, báo trước 9:00  Ms: Quyên: 01676857089 để chuẩn bị</t>
   </si>
   <si>
@@ -114,7 +112,10 @@
     <t>Note</t>
   </si>
   <si>
-    <t>Điều hành ký</t>
+    <t xml:space="preserve">Guide's Salary                                         </t>
+  </si>
+  <si>
+    <t>Điều hành ký lương</t>
   </si>
 </sst>
 </file>
@@ -509,7 +510,35 @@
     <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="12" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="12" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -539,34 +568,10 @@
     <xf numFmtId="0" fontId="4" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="12" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
@@ -598,10 +603,6 @@
       <alignment horizontal="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="12" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -945,7 +946,7 @@
   <dimension ref="A1:AA28"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B19" sqref="B19"/>
+      <selection activeCell="L8" sqref="L8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1411,17 +1412,17 @@
       <c r="B1" s="2"/>
       <c r="C1" s="2"/>
       <c r="D1" s="2"/>
-      <c r="E1" s="69"/>
-      <c r="F1" s="69"/>
-      <c r="G1" s="69"/>
-      <c r="H1" s="40">
+      <c r="E1" s="40"/>
+      <c r="F1" s="40"/>
+      <c r="G1" s="40"/>
+      <c r="H1" s="61">
         <v>40156</v>
       </c>
-      <c r="I1" s="40"/>
-      <c r="J1" s="68" t="s">
-        <v>16</v>
-      </c>
-      <c r="K1" s="68"/>
+      <c r="I1" s="61"/>
+      <c r="J1" s="60" t="s">
+        <v>13</v>
+      </c>
+      <c r="K1" s="60"/>
     </row>
     <row r="2" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A2" s="2"/>
@@ -1439,14 +1440,14 @@
     <row r="3" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A3" s="2"/>
       <c r="B3" s="2" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="C3" s="2"/>
       <c r="D3" s="15"/>
       <c r="E3" s="15"/>
       <c r="F3" s="15"/>
       <c r="G3" s="23" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="H3" s="15"/>
       <c r="I3" s="38"/>
@@ -1463,7 +1464,7 @@
       <c r="E4" s="15"/>
       <c r="F4" s="15"/>
       <c r="G4" s="23" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="H4" s="15"/>
       <c r="I4" s="2"/>
@@ -1473,14 +1474,14 @@
     <row r="5" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A5" s="2"/>
       <c r="B5" s="2" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="C5" s="2"/>
       <c r="D5" s="24"/>
       <c r="E5" s="24"/>
       <c r="F5" s="24"/>
       <c r="G5" s="23" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="H5" s="15"/>
       <c r="I5" s="2"/>
@@ -1488,57 +1489,57 @@
       <c r="K5" s="21"/>
     </row>
     <row r="6" spans="1:27" x14ac:dyDescent="0.2">
-      <c r="A6" s="41" t="s">
+      <c r="A6" s="51" t="s">
+        <v>6</v>
+      </c>
+      <c r="B6" s="52" t="s">
+        <v>1</v>
+      </c>
+      <c r="C6" s="53"/>
+      <c r="D6" s="56" t="s">
+        <v>7</v>
+      </c>
+      <c r="E6" s="56"/>
+      <c r="F6" s="56"/>
+      <c r="G6" s="57" t="s">
+        <v>16</v>
+      </c>
+      <c r="H6" s="51" t="s">
+        <v>2</v>
+      </c>
+      <c r="I6" s="57" t="s">
+        <v>8</v>
+      </c>
+      <c r="J6" s="58" t="s">
+        <v>24</v>
+      </c>
+      <c r="K6" s="51" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="7" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="A7" s="51"/>
+      <c r="B7" s="54"/>
+      <c r="C7" s="55"/>
+      <c r="D7" s="34" t="s">
         <v>9</v>
       </c>
-      <c r="B6" s="42" t="s">
-        <v>1</v>
-      </c>
-      <c r="C6" s="43"/>
-      <c r="D6" s="46" t="s">
+      <c r="E7" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="E6" s="46"/>
-      <c r="F6" s="46"/>
-      <c r="G6" s="47" t="s">
-        <v>19</v>
-      </c>
-      <c r="H6" s="41" t="s">
-        <v>2</v>
-      </c>
-      <c r="I6" s="47" t="s">
+      <c r="F7" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="J6" s="48" t="s">
-        <v>28</v>
-      </c>
-      <c r="K6" s="41" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="7" spans="1:27" x14ac:dyDescent="0.2">
-      <c r="A7" s="41"/>
-      <c r="B7" s="44"/>
-      <c r="C7" s="45"/>
-      <c r="D7" s="34" t="s">
-        <v>12</v>
-      </c>
-      <c r="E7" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="F7" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="G7" s="47"/>
-      <c r="H7" s="41"/>
-      <c r="I7" s="47"/>
-      <c r="J7" s="49"/>
-      <c r="K7" s="41"/>
+      <c r="G7" s="57"/>
+      <c r="H7" s="51"/>
+      <c r="I7" s="57"/>
+      <c r="J7" s="59"/>
+      <c r="K7" s="51"/>
     </row>
     <row r="8" spans="1:27" s="27" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A8" s="25"/>
-      <c r="B8" s="57"/>
-      <c r="C8" s="58"/>
+      <c r="B8" s="48"/>
+      <c r="C8" s="49"/>
       <c r="D8" s="25"/>
       <c r="E8" s="25"/>
       <c r="F8" s="25"/>
@@ -1552,7 +1553,7 @@
     <row r="9" spans="1:27" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A9" s="16"/>
       <c r="B9" s="29" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="C9" s="30"/>
       <c r="D9" s="30"/>
@@ -1592,17 +1593,17 @@
       <c r="I11" s="35" t="s">
         <v>25</v>
       </c>
-      <c r="J11" s="59" t="s">
-        <v>29</v>
-      </c>
-      <c r="K11" s="59"/>
+      <c r="J11" s="50" t="s">
+        <v>26</v>
+      </c>
+      <c r="K11" s="50"/>
     </row>
     <row r="12" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A12" s="7">
         <v>1</v>
       </c>
       <c r="B12" s="33" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="C12" s="33"/>
       <c r="D12" s="16"/>
@@ -1610,18 +1611,16 @@
       <c r="F12" s="16"/>
       <c r="G12" s="11"/>
       <c r="H12" s="11"/>
-      <c r="I12" s="36" t="s">
-        <v>5</v>
-      </c>
-      <c r="J12" s="50"/>
-      <c r="K12" s="51"/>
+      <c r="I12" s="36"/>
+      <c r="J12" s="41"/>
+      <c r="K12" s="42"/>
     </row>
     <row r="13" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A13" s="7">
         <v>2</v>
       </c>
       <c r="B13" s="18" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="C13" s="18"/>
       <c r="D13" s="1"/>
@@ -1629,11 +1628,9 @@
       <c r="F13" s="16"/>
       <c r="G13" s="1"/>
       <c r="H13" s="1"/>
-      <c r="I13" s="36" t="s">
-        <v>6</v>
-      </c>
-      <c r="J13" s="52"/>
-      <c r="K13" s="53"/>
+      <c r="I13" s="36"/>
+      <c r="J13" s="43"/>
+      <c r="K13" s="44"/>
     </row>
     <row r="14" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A14" s="7"/>
@@ -1644,26 +1641,24 @@
       <c r="F14" s="16"/>
       <c r="G14" s="1"/>
       <c r="H14" s="1"/>
-      <c r="I14" s="36" t="s">
-        <v>7</v>
-      </c>
-      <c r="J14" s="52"/>
-      <c r="K14" s="53"/>
+      <c r="I14" s="36"/>
+      <c r="J14" s="43"/>
+      <c r="K14" s="44"/>
     </row>
     <row r="15" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A15" s="14"/>
       <c r="B15" s="6"/>
       <c r="C15" s="6"/>
-      <c r="D15" s="56"/>
-      <c r="E15" s="56"/>
-      <c r="F15" s="56"/>
-      <c r="G15" s="56"/>
+      <c r="D15" s="47"/>
+      <c r="E15" s="47"/>
+      <c r="F15" s="47"/>
+      <c r="G15" s="47"/>
       <c r="H15" s="16"/>
       <c r="I15" s="37" t="s">
-        <v>8</v>
-      </c>
-      <c r="J15" s="54"/>
-      <c r="K15" s="55"/>
+        <v>5</v>
+      </c>
+      <c r="J15" s="45"/>
+      <c r="K15" s="46"/>
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.2">
       <c r="I18" s="5"/>
@@ -1775,6 +1770,8 @@
     </row>
   </sheetData>
   <mergeCells count="14">
+    <mergeCell ref="J1:K1"/>
+    <mergeCell ref="H1:I1"/>
     <mergeCell ref="J12:K15"/>
     <mergeCell ref="D15:G15"/>
     <mergeCell ref="B8:C8"/>
@@ -1787,8 +1784,6 @@
     <mergeCell ref="I6:I7"/>
     <mergeCell ref="J6:J7"/>
     <mergeCell ref="K6:K7"/>
-    <mergeCell ref="J1:K1"/>
-    <mergeCell ref="H1:I1"/>
   </mergeCells>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="landscape" r:id="rId1"/>
@@ -1821,97 +1816,97 @@
     <col min="12" max="16384" width="9.140625" style="19"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="118.5" customHeight="1" x14ac:dyDescent="1.25">
-      <c r="A1" s="62" t="s">
-        <v>16</v>
-      </c>
-      <c r="B1" s="62"/>
-      <c r="C1" s="62"/>
-      <c r="D1" s="62"/>
-      <c r="E1" s="62"/>
-      <c r="F1" s="62"/>
-      <c r="G1" s="62"/>
-      <c r="H1" s="62"/>
-      <c r="I1" s="62"/>
-      <c r="J1" s="62"/>
-      <c r="K1" s="62"/>
-    </row>
-    <row r="2" spans="1:11" ht="41.25" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A2" s="63" t="s">
-        <v>24</v>
-      </c>
-      <c r="B2" s="63"/>
-      <c r="C2" s="63"/>
-      <c r="D2" s="63"/>
-      <c r="E2" s="63"/>
-      <c r="F2" s="63"/>
-      <c r="G2" s="63"/>
-      <c r="H2" s="63"/>
-      <c r="I2" s="63"/>
-      <c r="J2" s="63"/>
-      <c r="K2" s="63"/>
+    <row r="1" spans="1:11" ht="118.5" customHeight="1" x14ac:dyDescent="1.2">
+      <c r="A1" s="64" t="s">
+        <v>13</v>
+      </c>
+      <c r="B1" s="64"/>
+      <c r="C1" s="64"/>
+      <c r="D1" s="64"/>
+      <c r="E1" s="64"/>
+      <c r="F1" s="64"/>
+      <c r="G1" s="64"/>
+      <c r="H1" s="64"/>
+      <c r="I1" s="64"/>
+      <c r="J1" s="64"/>
+      <c r="K1" s="64"/>
+    </row>
+    <row r="2" spans="1:11" ht="41.25" customHeight="1" x14ac:dyDescent="0.5">
+      <c r="A2" s="65" t="s">
+        <v>21</v>
+      </c>
+      <c r="B2" s="65"/>
+      <c r="C2" s="65"/>
+      <c r="D2" s="65"/>
+      <c r="E2" s="65"/>
+      <c r="F2" s="65"/>
+      <c r="G2" s="65"/>
+      <c r="H2" s="65"/>
+      <c r="I2" s="65"/>
+      <c r="J2" s="65"/>
+      <c r="K2" s="65"/>
     </row>
     <row r="3" spans="1:11" ht="301.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="65"/>
-      <c r="B3" s="65"/>
-      <c r="C3" s="65"/>
-      <c r="D3" s="65"/>
-      <c r="E3" s="65"/>
-      <c r="F3" s="65"/>
-      <c r="G3" s="65"/>
-      <c r="H3" s="65"/>
-      <c r="I3" s="65"/>
-      <c r="J3" s="65"/>
-      <c r="K3" s="65"/>
+      <c r="A3" s="67"/>
+      <c r="B3" s="67"/>
+      <c r="C3" s="67"/>
+      <c r="D3" s="67"/>
+      <c r="E3" s="67"/>
+      <c r="F3" s="67"/>
+      <c r="G3" s="67"/>
+      <c r="H3" s="67"/>
+      <c r="I3" s="67"/>
+      <c r="J3" s="67"/>
+      <c r="K3" s="67"/>
     </row>
     <row r="4" spans="1:11" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="66"/>
-      <c r="B4" s="67"/>
-      <c r="C4" s="67"/>
-      <c r="D4" s="67"/>
-      <c r="E4" s="67"/>
-      <c r="F4" s="67"/>
-      <c r="G4" s="67"/>
-      <c r="H4" s="67"/>
-      <c r="I4" s="67"/>
-      <c r="J4" s="67"/>
-      <c r="K4" s="67"/>
+      <c r="A4" s="68"/>
+      <c r="B4" s="69"/>
+      <c r="C4" s="69"/>
+      <c r="D4" s="69"/>
+      <c r="E4" s="69"/>
+      <c r="F4" s="69"/>
+      <c r="G4" s="69"/>
+      <c r="H4" s="69"/>
+      <c r="I4" s="69"/>
+      <c r="J4" s="69"/>
+      <c r="K4" s="69"/>
     </row>
     <row r="5" spans="1:11" ht="46.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="20" t="s">
         <v>0</v>
       </c>
-      <c r="B5" s="64"/>
-      <c r="C5" s="60"/>
+      <c r="B5" s="66"/>
+      <c r="C5" s="62"/>
       <c r="D5" s="20" t="s">
         <v>2</v>
       </c>
-      <c r="E5" s="61"/>
-      <c r="F5" s="61"/>
-      <c r="G5" s="61"/>
-      <c r="H5" s="61"/>
+      <c r="E5" s="63"/>
+      <c r="F5" s="63"/>
+      <c r="G5" s="63"/>
+      <c r="H5" s="63"/>
       <c r="I5" s="20" t="s">
-        <v>23</v>
-      </c>
-      <c r="J5" s="60"/>
-      <c r="K5" s="60"/>
+        <v>20</v>
+      </c>
+      <c r="J5" s="62"/>
+      <c r="K5" s="62"/>
     </row>
     <row r="6" spans="1:11" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="20" t="s">
-        <v>22</v>
-      </c>
-      <c r="B6" s="64"/>
-      <c r="C6" s="60"/>
+        <v>19</v>
+      </c>
+      <c r="B6" s="66"/>
+      <c r="C6" s="62"/>
       <c r="D6" s="20"/>
-      <c r="E6" s="61"/>
-      <c r="F6" s="61"/>
-      <c r="G6" s="61"/>
-      <c r="H6" s="61"/>
+      <c r="E6" s="63"/>
+      <c r="F6" s="63"/>
+      <c r="G6" s="63"/>
+      <c r="H6" s="63"/>
       <c r="I6" s="20" t="s">
-        <v>21</v>
-      </c>
-      <c r="J6" s="60"/>
-      <c r="K6" s="60"/>
+        <v>18</v>
+      </c>
+      <c r="J6" s="62"/>
+      <c r="K6" s="62"/>
     </row>
   </sheetData>
   <sheetProtection selectLockedCells="1"/>

</xml_diff>